<commit_message>
Agregue los cuestionarios de la unidad 4 hechos a último momento
</commit_message>
<xml_diff>
--- a/Estadística aplicada a los negocios - Calificaciones finales - 1er cuatrimestre 2025.xlsx
+++ b/Estadística aplicada a los negocios - Calificaciones finales - 1er cuatrimestre 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juangallardo/Desktop/Facu/UTN/Estadistica aplicada a negocios/1er Cuatrimestre/Notas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405A4A1A-5211-514F-8952-47A40705616D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37145A9E-FC2C-9C43-960E-A9D5194C4120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="-1100" windowWidth="28800" windowHeight="16540" xr2:uid="{BD3AB91B-0124-FD42-AF99-EC8FFD8D06CC}"/>
+    <workbookView xWindow="-28800" yWindow="-1100" windowWidth="28800" windowHeight="17500" xr2:uid="{BD3AB91B-0124-FD42-AF99-EC8FFD8D06CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Calificaciones - En Limpio" sheetId="2" r:id="rId1"/>
@@ -6113,8 +6113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3E5BC9-1D37-D445-9104-0B358164814E}">
   <dimension ref="A1:AB524"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A493" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -6122,7 +6122,6 @@
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" style="5" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="3" customWidth="1"/>
@@ -6270,13 +6269,13 @@
         <v>19</v>
       </c>
       <c r="E5" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F5">
         <v>8</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
@@ -6324,13 +6323,13 @@
         <v>27</v>
       </c>
       <c r="E7" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F7">
         <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
@@ -6405,7 +6404,7 @@
         <v>39</v>
       </c>
       <c r="E10" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -6559,13 +6558,13 @@
         <v>63</v>
       </c>
       <c r="E16" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F16">
         <v>8</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6697,7 +6696,7 @@
         <v>83</v>
       </c>
       <c r="E22" s="5">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F22">
         <v>10</v>
@@ -7019,7 +7018,7 @@
         <v>139</v>
       </c>
       <c r="E36" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F36">
         <v>10</v>
@@ -7111,13 +7110,13 @@
         <v>155</v>
       </c>
       <c r="E40" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F40">
         <v>8</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -7134,7 +7133,7 @@
         <v>159</v>
       </c>
       <c r="E41" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F41">
         <v>8</v>
@@ -7157,13 +7156,13 @@
         <v>163</v>
       </c>
       <c r="E42" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F42">
         <v>9</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -7180,7 +7179,7 @@
         <v>167</v>
       </c>
       <c r="E43" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F43">
         <v>9</v>
@@ -7272,7 +7271,7 @@
         <v>183</v>
       </c>
       <c r="E47" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F47">
         <v>10</v>
@@ -7410,7 +7409,7 @@
         <v>207</v>
       </c>
       <c r="E53" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F53">
         <v>9</v>
@@ -7456,7 +7455,7 @@
         <v>215</v>
       </c>
       <c r="E55" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F55">
         <v>9</v>
@@ -7548,7 +7547,7 @@
         <v>231</v>
       </c>
       <c r="E59" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F59">
         <v>9</v>
@@ -7663,7 +7662,7 @@
         <v>251</v>
       </c>
       <c r="E64" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F64">
         <v>9</v>
@@ -7686,13 +7685,13 @@
         <v>255</v>
       </c>
       <c r="E65" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F65">
         <v>10</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -7709,7 +7708,7 @@
         <v>259</v>
       </c>
       <c r="E66" s="5">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="F66">
         <v>9</v>
@@ -7939,7 +7938,7 @@
         <v>299</v>
       </c>
       <c r="E76" s="5">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="F76">
         <v>10</v>
@@ -7962,7 +7961,7 @@
         <v>302</v>
       </c>
       <c r="E77" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F77">
         <v>9</v>
@@ -8054,7 +8053,7 @@
         <v>315</v>
       </c>
       <c r="E81" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F81">
         <v>2</v>
@@ -8261,13 +8260,13 @@
         <v>350</v>
       </c>
       <c r="E90" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F90">
         <v>9</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -8445,7 +8444,7 @@
         <v>382</v>
       </c>
       <c r="E98" s="5">
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="F98">
         <v>8</v>
@@ -8537,13 +8536,13 @@
         <v>397</v>
       </c>
       <c r="E102" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F102">
         <v>10</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -8790,7 +8789,7 @@
         <v>437</v>
       </c>
       <c r="E113" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F113">
         <v>9</v>
@@ -8928,7 +8927,7 @@
         <v>459</v>
       </c>
       <c r="E119" s="5">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="F119">
         <v>9</v>
@@ -8951,7 +8950,7 @@
         <v>463</v>
       </c>
       <c r="E120" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F120">
         <v>10</v>
@@ -8974,7 +8973,7 @@
         <v>467</v>
       </c>
       <c r="E121" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F121">
         <v>4</v>
@@ -8997,7 +8996,7 @@
         <v>471</v>
       </c>
       <c r="E122" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F122">
         <v>9</v>
@@ -9020,7 +9019,7 @@
         <v>475</v>
       </c>
       <c r="E123" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F123">
         <v>10</v>
@@ -9089,13 +9088,13 @@
         <v>487</v>
       </c>
       <c r="E126" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F126">
         <v>10</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -9158,13 +9157,13 @@
         <v>497</v>
       </c>
       <c r="E129" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F129">
         <v>8</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -9273,7 +9272,7 @@
         <v>514</v>
       </c>
       <c r="E134" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F134">
         <v>9</v>
@@ -9342,7 +9341,7 @@
         <v>524</v>
       </c>
       <c r="E137" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F137">
         <v>9</v>
@@ -9365,13 +9364,13 @@
         <v>528</v>
       </c>
       <c r="E138" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F138">
         <v>9</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -9434,7 +9433,7 @@
         <v>539</v>
       </c>
       <c r="E141" s="5">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="F141">
         <v>9</v>
@@ -9480,7 +9479,7 @@
         <v>546</v>
       </c>
       <c r="E143" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F143">
         <v>10</v>
@@ -9549,7 +9548,7 @@
         <v>558</v>
       </c>
       <c r="E146" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F146">
         <v>8</v>
@@ -9572,13 +9571,13 @@
         <v>562</v>
       </c>
       <c r="E147" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F147">
         <v>10</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -9595,7 +9594,7 @@
         <v>566</v>
       </c>
       <c r="E148" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F148">
         <v>9</v>
@@ -9802,7 +9801,7 @@
         <v>598</v>
       </c>
       <c r="E157" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F157">
         <v>4</v>
@@ -9894,13 +9893,13 @@
         <v>613</v>
       </c>
       <c r="E161" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F161">
         <v>9</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -9940,7 +9939,7 @@
         <v>619</v>
       </c>
       <c r="E163" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F163">
         <v>7</v>
@@ -9963,13 +9962,13 @@
         <v>623</v>
       </c>
       <c r="E164" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F164">
         <v>8</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -10124,7 +10123,7 @@
         <v>644</v>
       </c>
       <c r="E171" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F171">
         <v>9</v>
@@ -10285,7 +10284,7 @@
         <v>670</v>
       </c>
       <c r="E178" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F178">
         <v>4</v>
@@ -10308,7 +10307,7 @@
         <v>674</v>
       </c>
       <c r="E179" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F179">
         <v>10</v>
@@ -10331,7 +10330,7 @@
         <v>678</v>
       </c>
       <c r="E180" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F180">
         <v>9</v>
@@ -10400,7 +10399,7 @@
         <v>689</v>
       </c>
       <c r="E183" s="5">
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="F183">
         <v>10</v>
@@ -10423,13 +10422,13 @@
         <v>692</v>
       </c>
       <c r="E184" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F184">
         <v>8</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -10446,13 +10445,13 @@
         <v>696</v>
       </c>
       <c r="E185" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F185">
         <v>10</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -10538,13 +10537,13 @@
         <v>710</v>
       </c>
       <c r="E189" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F189">
         <v>9</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -10630,7 +10629,7 @@
         <v>725</v>
       </c>
       <c r="E193" s="5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F193">
         <v>10</v>
@@ -10745,7 +10744,7 @@
         <v>741</v>
       </c>
       <c r="E198" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F198">
         <v>8</v>
@@ -10814,7 +10813,7 @@
         <v>752</v>
       </c>
       <c r="E201" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F201">
         <v>9</v>
@@ -10906,13 +10905,13 @@
         <v>766</v>
       </c>
       <c r="E205" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F205">
         <v>9</v>
       </c>
       <c r="G205" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -11067,7 +11066,7 @@
         <v>791</v>
       </c>
       <c r="E212" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F212">
         <v>9</v>
@@ -11090,7 +11089,7 @@
         <v>795</v>
       </c>
       <c r="E213" s="5">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F213">
         <v>9</v>
@@ -11113,7 +11112,7 @@
         <v>799</v>
       </c>
       <c r="E214" s="5">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="F214">
         <v>10</v>
@@ -11159,7 +11158,7 @@
         <v>805</v>
       </c>
       <c r="E216" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F216">
         <v>4</v>
@@ -11182,7 +11181,7 @@
         <v>808</v>
       </c>
       <c r="E217" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F217">
         <v>8</v>
@@ -11205,7 +11204,7 @@
         <v>811</v>
       </c>
       <c r="E218" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F218">
         <v>9</v>
@@ -11389,7 +11388,7 @@
         <v>834</v>
       </c>
       <c r="E226" s="5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F226">
         <v>9</v>
@@ -11435,7 +11434,7 @@
         <v>841</v>
       </c>
       <c r="E228" s="5">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="F228">
         <v>9</v>
@@ -11527,7 +11526,7 @@
         <v>856</v>
       </c>
       <c r="E232" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F232">
         <v>9</v>
@@ -11550,13 +11549,13 @@
         <v>860</v>
       </c>
       <c r="E233" s="5">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="F233">
         <v>9</v>
       </c>
       <c r="G233" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -11573,7 +11572,7 @@
         <v>863</v>
       </c>
       <c r="E234" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F234">
         <v>9</v>
@@ -11688,7 +11687,7 @@
         <v>881</v>
       </c>
       <c r="E239" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F239">
         <v>10</v>
@@ -11780,7 +11779,7 @@
         <v>894</v>
       </c>
       <c r="E243" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F243">
         <v>10</v>
@@ -11826,7 +11825,7 @@
         <v>901</v>
       </c>
       <c r="E245" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F245">
         <v>9</v>
@@ -11964,7 +11963,7 @@
         <v>923</v>
       </c>
       <c r="E251" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F251">
         <v>10</v>
@@ -12010,7 +12009,7 @@
         <v>929</v>
       </c>
       <c r="E253" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F253">
         <v>10</v>
@@ -12194,7 +12193,7 @@
         <v>957</v>
       </c>
       <c r="E261" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F261">
         <v>9</v>
@@ -12378,7 +12377,7 @@
         <v>986</v>
       </c>
       <c r="E269" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F269">
         <v>9</v>
@@ -12424,7 +12423,7 @@
         <v>993</v>
       </c>
       <c r="E271" s="5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F271">
         <v>9</v>
@@ -12516,13 +12515,13 @@
         <v>1009</v>
       </c>
       <c r="E275" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F275">
         <v>9</v>
       </c>
       <c r="G275" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
@@ -12654,13 +12653,13 @@
         <v>1031</v>
       </c>
       <c r="E281" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F281">
         <v>10</v>
       </c>
       <c r="G281" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
@@ -12677,7 +12676,7 @@
         <v>1035</v>
       </c>
       <c r="E282" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F282">
         <v>9</v>
@@ -12700,7 +12699,7 @@
         <v>1039</v>
       </c>
       <c r="E283" s="5">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="F283">
         <v>9</v>
@@ -12723,7 +12722,7 @@
         <v>1042</v>
       </c>
       <c r="E284" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F284">
         <v>10</v>
@@ -12907,7 +12906,7 @@
         <v>1070</v>
       </c>
       <c r="E292" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F292">
         <v>9</v>
@@ -12953,13 +12952,13 @@
         <v>1078</v>
       </c>
       <c r="E294" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F294">
         <v>9</v>
       </c>
       <c r="G294" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
@@ -12999,7 +12998,7 @@
         <v>1085</v>
       </c>
       <c r="E296" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F296">
         <v>8</v>
@@ -13137,7 +13136,7 @@
         <v>1108</v>
       </c>
       <c r="E302" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F302">
         <v>9</v>
@@ -13436,7 +13435,7 @@
         <v>1153</v>
       </c>
       <c r="E315" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F315">
         <v>10</v>
@@ -13459,7 +13458,7 @@
         <v>1156</v>
       </c>
       <c r="E316" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F316">
         <v>10</v>
@@ -13643,7 +13642,7 @@
         <v>1184</v>
       </c>
       <c r="E324" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F324">
         <v>10</v>
@@ -13735,13 +13734,13 @@
         <v>1198</v>
       </c>
       <c r="E328" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F328">
         <v>10</v>
       </c>
       <c r="G328" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.25">
@@ -13758,7 +13757,7 @@
         <v>1201</v>
       </c>
       <c r="E329" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F329">
         <v>10</v>
@@ -13827,7 +13826,7 @@
         <v>1213</v>
       </c>
       <c r="E332" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F332">
         <v>10</v>
@@ -13850,7 +13849,7 @@
         <v>1217</v>
       </c>
       <c r="E333" s="5">
-        <v>0.75</v>
+        <v>0.875</v>
       </c>
       <c r="F333">
         <v>9</v>
@@ -13965,7 +13964,7 @@
         <v>1233</v>
       </c>
       <c r="E338" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F338">
         <v>5</v>
@@ -13988,7 +13987,7 @@
         <v>1236</v>
       </c>
       <c r="E339" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F339">
         <v>9</v>
@@ -14057,7 +14056,7 @@
         <v>1245</v>
       </c>
       <c r="E342" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F342">
         <v>10</v>
@@ -14195,7 +14194,7 @@
         <v>1268</v>
       </c>
       <c r="E348" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F348">
         <v>8</v>
@@ -14264,7 +14263,7 @@
         <v>1278</v>
       </c>
       <c r="E351" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F351">
         <v>9</v>
@@ -14310,7 +14309,7 @@
         <v>1284</v>
       </c>
       <c r="E353" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F353">
         <v>9</v>
@@ -14356,13 +14355,13 @@
         <v>1291</v>
       </c>
       <c r="E355" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F355">
         <v>10</v>
       </c>
       <c r="G355" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="356" spans="1:7" x14ac:dyDescent="0.25">
@@ -14379,13 +14378,13 @@
         <v>1294</v>
       </c>
       <c r="E356" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F356">
         <v>9</v>
       </c>
       <c r="G356" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="357" spans="1:7" x14ac:dyDescent="0.25">
@@ -14402,7 +14401,7 @@
         <v>1297</v>
       </c>
       <c r="E357" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F357">
         <v>10</v>
@@ -14494,7 +14493,7 @@
         <v>1310</v>
       </c>
       <c r="E361" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F361">
         <v>9</v>
@@ -14517,7 +14516,7 @@
         <v>1312</v>
       </c>
       <c r="E362" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F362">
         <v>10</v>
@@ -14540,7 +14539,7 @@
         <v>1316</v>
       </c>
       <c r="E363" s="5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F363">
         <v>10</v>
@@ -14563,7 +14562,7 @@
         <v>1320</v>
       </c>
       <c r="E364" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F364">
         <v>10</v>
@@ -14701,7 +14700,7 @@
         <v>1342</v>
       </c>
       <c r="E370" s="5">
-        <v>0.875</v>
+        <v>1</v>
       </c>
       <c r="F370">
         <v>9</v>
@@ -14724,13 +14723,13 @@
         <v>1346</v>
       </c>
       <c r="E371" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F371">
         <v>9</v>
       </c>
       <c r="G371" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
@@ -14793,7 +14792,7 @@
         <v>1355</v>
       </c>
       <c r="E374" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F374">
         <v>10</v>
@@ -14862,7 +14861,7 @@
         <v>1366</v>
       </c>
       <c r="E377" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F377">
         <v>10</v>
@@ -15023,7 +15022,7 @@
         <v>1387</v>
       </c>
       <c r="E384" s="5">
-        <v>0.125</v>
+        <v>0.375</v>
       </c>
       <c r="F384">
         <v>10</v>
@@ -15046,7 +15045,7 @@
         <v>1391</v>
       </c>
       <c r="E385" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F385">
         <v>10</v>
@@ -15069,13 +15068,13 @@
         <v>1394</v>
       </c>
       <c r="E386" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F386">
         <v>10</v>
       </c>
       <c r="G386" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="387" spans="1:7" x14ac:dyDescent="0.25">
@@ -15368,7 +15367,7 @@
         <v>1437</v>
       </c>
       <c r="E399" s="5">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="F399">
         <v>8</v>
@@ -15437,13 +15436,13 @@
         <v>1447</v>
       </c>
       <c r="E402" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F402">
         <v>9</v>
       </c>
       <c r="G402" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="403" spans="1:7" x14ac:dyDescent="0.25">
@@ -15598,7 +15597,7 @@
         <v>1474</v>
       </c>
       <c r="E409" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F409">
         <v>9</v>
@@ -15690,7 +15689,7 @@
         <v>1489</v>
       </c>
       <c r="E413" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F413">
         <v>9</v>
@@ -15736,7 +15735,7 @@
         <v>1497</v>
       </c>
       <c r="E415" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F415">
         <v>10</v>
@@ -15782,7 +15781,7 @@
         <v>1502</v>
       </c>
       <c r="E417" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F417">
         <v>9</v>
@@ -15874,7 +15873,7 @@
         <v>1513</v>
       </c>
       <c r="E421" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F421">
         <v>10</v>
@@ -16035,7 +16034,7 @@
         <v>1535</v>
       </c>
       <c r="E428" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F428">
         <v>10</v>
@@ -16058,7 +16057,7 @@
         <v>1538</v>
       </c>
       <c r="E429" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F429">
         <v>3</v>
@@ -16104,13 +16103,13 @@
         <v>1544</v>
       </c>
       <c r="E431" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F431">
         <v>9</v>
       </c>
       <c r="G431" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="432" spans="1:7" x14ac:dyDescent="0.25">
@@ -16380,7 +16379,7 @@
         <v>1588</v>
       </c>
       <c r="E443" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F443">
         <v>9</v>
@@ -16403,13 +16402,13 @@
         <v>1592</v>
       </c>
       <c r="E444" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F444">
         <v>9</v>
       </c>
       <c r="G444" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="445" spans="1:7" x14ac:dyDescent="0.25">
@@ -16426,13 +16425,13 @@
         <v>1596</v>
       </c>
       <c r="E445" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F445">
         <v>10</v>
       </c>
       <c r="G445" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="446" spans="1:7" x14ac:dyDescent="0.25">
@@ -16472,7 +16471,7 @@
         <v>1603</v>
       </c>
       <c r="E447" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F447">
         <v>8</v>
@@ -16656,13 +16655,13 @@
         <v>1632</v>
       </c>
       <c r="E455" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F455">
         <v>10</v>
       </c>
       <c r="G455" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="456" spans="1:7" x14ac:dyDescent="0.25">
@@ -16794,7 +16793,7 @@
         <v>1654</v>
       </c>
       <c r="E461" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F461">
         <v>8</v>
@@ -16817,13 +16816,13 @@
         <v>1657</v>
       </c>
       <c r="E462" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F462">
         <v>10</v>
       </c>
       <c r="G462" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="463" spans="1:7" x14ac:dyDescent="0.25">
@@ -16909,13 +16908,13 @@
         <v>1670</v>
       </c>
       <c r="E466" s="5">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="F466">
         <v>8</v>
       </c>
       <c r="G466" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="467" spans="1:7" x14ac:dyDescent="0.25">
@@ -16932,13 +16931,13 @@
         <v>1674</v>
       </c>
       <c r="E467" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F467">
         <v>8</v>
       </c>
       <c r="G467" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="468" spans="1:7" x14ac:dyDescent="0.25">
@@ -17024,7 +17023,7 @@
         <v>1688</v>
       </c>
       <c r="E471" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F471">
         <v>9</v>
@@ -17116,7 +17115,7 @@
         <v>1701</v>
       </c>
       <c r="E475" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F475">
         <v>5</v>
@@ -17208,13 +17207,13 @@
         <v>1714</v>
       </c>
       <c r="E479" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F479">
         <v>9</v>
       </c>
       <c r="G479" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="480" spans="1:7" x14ac:dyDescent="0.25">
@@ -17277,7 +17276,7 @@
         <v>1724</v>
       </c>
       <c r="E482" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F482">
         <v>8</v>
@@ -17369,7 +17368,7 @@
         <v>1738</v>
       </c>
       <c r="E486" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F486">
         <v>10</v>
@@ -17484,7 +17483,7 @@
         <v>1755</v>
       </c>
       <c r="E491" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F491">
         <v>7</v>
@@ -17530,13 +17529,13 @@
         <v>1762</v>
       </c>
       <c r="E493" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F493">
         <v>8</v>
       </c>
       <c r="G493" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="494" spans="1:7" x14ac:dyDescent="0.25">
@@ -17599,7 +17598,7 @@
         <v>1773</v>
       </c>
       <c r="E496" s="5">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F496">
         <v>10</v>
@@ -17622,7 +17621,7 @@
         <v>1776</v>
       </c>
       <c r="E497" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F497">
         <v>10</v>
@@ -17645,7 +17644,7 @@
         <v>1780</v>
       </c>
       <c r="E498" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F498">
         <v>10</v>
@@ -17737,7 +17736,7 @@
         <v>1795</v>
       </c>
       <c r="E502" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F502">
         <v>10</v>
@@ -17760,7 +17759,7 @@
         <v>1799</v>
       </c>
       <c r="E503" s="5">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="F503">
         <v>9</v>
@@ -17852,7 +17851,7 @@
         <v>1815</v>
       </c>
       <c r="E507" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F507">
         <v>10</v>
@@ -17921,7 +17920,7 @@
         <v>1826</v>
       </c>
       <c r="E510" s="5">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F510">
         <v>10</v>
@@ -17944,13 +17943,13 @@
         <v>1829</v>
       </c>
       <c r="E511" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F511">
         <v>8</v>
       </c>
       <c r="G511" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="512" spans="1:7" x14ac:dyDescent="0.25">
@@ -17967,7 +17966,7 @@
         <v>1832</v>
       </c>
       <c r="E512" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F512">
         <v>3</v>
@@ -18082,13 +18081,13 @@
         <v>1850</v>
       </c>
       <c r="E517" s="5">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F517">
         <v>10</v>
       </c>
       <c r="G517" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="518" spans="1:7" x14ac:dyDescent="0.25">
@@ -18128,7 +18127,7 @@
         <v>1857</v>
       </c>
       <c r="E519" s="5">
-        <v>0.625</v>
+        <v>0.875</v>
       </c>
       <c r="F519">
         <v>9</v>
@@ -18243,13 +18242,13 @@
         <v>1875</v>
       </c>
       <c r="E524" s="5">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="F524">
         <v>10</v>
       </c>
       <c r="G524" s="3" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>